<commit_message>
rename files and segment wald analysis sections
</commit_message>
<xml_diff>
--- a/figures/source/wald-register-space.xlsx
+++ b/figures/source/wald-register-space.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -118,7 +118,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -145,6 +145,14 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -258,7 +266,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -267,6 +275,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -661,14 +670,14 @@
   <dimension ref="A1:V89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
     <col min="2" max="2" width="2" customWidth="1"/>
-    <col min="3" max="3" width="4.5" customWidth="1"/>
+    <col min="3" max="3" width="4.5" style="8" customWidth="1"/>
     <col min="4" max="4" width="16.875" customWidth="1"/>
     <col min="5" max="5" width="19.125" customWidth="1"/>
     <col min="6" max="6" width="21.375" customWidth="1"/>
@@ -681,62 +690,62 @@
     <col min="17" max="17" width="39.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
-      <c r="D1" t="s">
+    <row r="1" spans="1:22" s="8" customFormat="1">
+      <c r="D1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="8" t="s">
         <v>30</v>
       </c>
     </row>
@@ -747,7 +756,7 @@
       <c r="B2">
         <v>8</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C2" s="8" t="str">
         <f>CONCATENATE(A2,B2)</f>
         <v>C8</v>
       </c>
@@ -759,7 +768,7 @@
       <c r="B3">
         <v>7</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C3" s="8" t="str">
         <f t="shared" ref="C3:C66" si="0">CONCATENATE(A3,B3)</f>
         <v>B7</v>
       </c>
@@ -771,7 +780,7 @@
       <c r="B4">
         <v>7</v>
       </c>
-      <c r="C4" t="str">
+      <c r="C4" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Bb7</v>
       </c>
@@ -783,7 +792,7 @@
       <c r="B5">
         <v>7</v>
       </c>
-      <c r="C5" t="str">
+      <c r="C5" s="8" t="str">
         <f t="shared" si="0"/>
         <v>A7</v>
       </c>
@@ -795,7 +804,7 @@
       <c r="B6">
         <v>7</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C6" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Ab7</v>
       </c>
@@ -807,7 +816,7 @@
       <c r="B7">
         <v>7</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" s="8" t="str">
         <f t="shared" si="0"/>
         <v>G7</v>
       </c>
@@ -819,7 +828,7 @@
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C8" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Gb7</v>
       </c>
@@ -831,7 +840,7 @@
       <c r="B9">
         <v>7</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" s="8" t="str">
         <f t="shared" si="0"/>
         <v>F7</v>
       </c>
@@ -843,7 +852,7 @@
       <c r="B10">
         <v>7</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C10" s="8" t="str">
         <f t="shared" si="0"/>
         <v>E7</v>
       </c>
@@ -855,7 +864,7 @@
       <c r="B11">
         <v>7</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Eb7</v>
       </c>
@@ -867,7 +876,7 @@
       <c r="B12">
         <v>7</v>
       </c>
-      <c r="C12" t="str">
+      <c r="C12" s="8" t="str">
         <f t="shared" si="0"/>
         <v>D7</v>
       </c>
@@ -879,7 +888,7 @@
       <c r="B13">
         <v>7</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Db7</v>
       </c>
@@ -892,7 +901,7 @@
       <c r="B14">
         <v>6</v>
       </c>
-      <c r="C14" t="str">
+      <c r="C14" s="8" t="str">
         <f t="shared" si="0"/>
         <v>C6</v>
       </c>
@@ -905,7 +914,7 @@
       <c r="B15">
         <v>6</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15" s="8" t="str">
         <f t="shared" si="0"/>
         <v>B6</v>
       </c>
@@ -918,7 +927,7 @@
       <c r="B16">
         <v>6</v>
       </c>
-      <c r="C16" t="str">
+      <c r="C16" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Bb6</v>
       </c>
@@ -932,7 +941,7 @@
       <c r="B17">
         <v>6</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" s="8" t="str">
         <f t="shared" si="0"/>
         <v>A6</v>
       </c>
@@ -946,7 +955,7 @@
       <c r="B18">
         <v>6</v>
       </c>
-      <c r="C18" t="str">
+      <c r="C18" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Ab6</v>
       </c>
@@ -960,7 +969,7 @@
       <c r="B19">
         <v>6</v>
       </c>
-      <c r="C19" t="str">
+      <c r="C19" s="8" t="str">
         <f t="shared" si="0"/>
         <v>G6</v>
       </c>
@@ -974,7 +983,7 @@
       <c r="B20">
         <v>6</v>
       </c>
-      <c r="C20" t="str">
+      <c r="C20" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Gb6</v>
       </c>
@@ -988,7 +997,7 @@
       <c r="B21">
         <v>6</v>
       </c>
-      <c r="C21" t="str">
+      <c r="C21" s="8" t="str">
         <f t="shared" si="0"/>
         <v>F6</v>
       </c>
@@ -1002,7 +1011,7 @@
       <c r="B22">
         <v>6</v>
       </c>
-      <c r="C22" t="str">
+      <c r="C22" s="8" t="str">
         <f t="shared" si="0"/>
         <v>E6</v>
       </c>
@@ -1017,7 +1026,7 @@
       <c r="B23">
         <v>6</v>
       </c>
-      <c r="C23" t="str">
+      <c r="C23" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Eb6</v>
       </c>
@@ -1033,7 +1042,7 @@
       <c r="B24">
         <v>6</v>
       </c>
-      <c r="C24" t="str">
+      <c r="C24" s="8" t="str">
         <f t="shared" si="0"/>
         <v>D6</v>
       </c>
@@ -1049,7 +1058,7 @@
       <c r="B25">
         <v>6</v>
       </c>
-      <c r="C25" t="str">
+      <c r="C25" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Db6</v>
       </c>
@@ -1065,7 +1074,7 @@
       <c r="B26">
         <v>5</v>
       </c>
-      <c r="C26" t="str">
+      <c r="C26" s="8" t="str">
         <f t="shared" si="0"/>
         <v>C5</v>
       </c>
@@ -1080,7 +1089,7 @@
       <c r="B27">
         <v>5</v>
       </c>
-      <c r="C27" t="str">
+      <c r="C27" s="8" t="str">
         <f t="shared" si="0"/>
         <v>B5</v>
       </c>
@@ -1095,7 +1104,7 @@
       <c r="B28">
         <v>5</v>
       </c>
-      <c r="C28" t="str">
+      <c r="C28" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Bb5</v>
       </c>
@@ -1111,7 +1120,7 @@
       <c r="B29">
         <v>5</v>
       </c>
-      <c r="C29" t="str">
+      <c r="C29" s="8" t="str">
         <f t="shared" si="0"/>
         <v>A5</v>
       </c>
@@ -1127,7 +1136,7 @@
       <c r="B30">
         <v>5</v>
       </c>
-      <c r="C30" t="str">
+      <c r="C30" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Ab5</v>
       </c>
@@ -1143,7 +1152,7 @@
       <c r="B31">
         <v>5</v>
       </c>
-      <c r="C31" t="str">
+      <c r="C31" s="8" t="str">
         <f t="shared" si="0"/>
         <v>G5</v>
       </c>
@@ -1158,7 +1167,7 @@
       <c r="B32">
         <v>5</v>
       </c>
-      <c r="C32" t="str">
+      <c r="C32" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Gb5</v>
       </c>
@@ -1173,7 +1182,7 @@
       <c r="B33">
         <v>5</v>
       </c>
-      <c r="C33" t="str">
+      <c r="C33" s="8" t="str">
         <f t="shared" si="0"/>
         <v>F5</v>
       </c>
@@ -1188,7 +1197,7 @@
       <c r="B34">
         <v>5</v>
       </c>
-      <c r="C34" t="str">
+      <c r="C34" s="8" t="str">
         <f t="shared" si="0"/>
         <v>E5</v>
       </c>
@@ -1203,7 +1212,7 @@
       <c r="B35">
         <v>5</v>
       </c>
-      <c r="C35" t="str">
+      <c r="C35" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Eb5</v>
       </c>
@@ -1218,7 +1227,7 @@
       <c r="B36">
         <v>5</v>
       </c>
-      <c r="C36" t="str">
+      <c r="C36" s="8" t="str">
         <f t="shared" si="0"/>
         <v>D5</v>
       </c>
@@ -1233,7 +1242,7 @@
       <c r="B37">
         <v>5</v>
       </c>
-      <c r="C37" t="str">
+      <c r="C37" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Db5</v>
       </c>
@@ -1248,7 +1257,7 @@
       <c r="B38">
         <v>4</v>
       </c>
-      <c r="C38" t="str">
+      <c r="C38" s="8" t="str">
         <f t="shared" si="0"/>
         <v>C4</v>
       </c>
@@ -1263,7 +1272,7 @@
       <c r="B39">
         <v>4</v>
       </c>
-      <c r="C39" t="str">
+      <c r="C39" s="8" t="str">
         <f t="shared" si="0"/>
         <v>B4</v>
       </c>
@@ -1278,7 +1287,7 @@
       <c r="B40">
         <v>4</v>
       </c>
-      <c r="C40" t="str">
+      <c r="C40" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Bb4</v>
       </c>
@@ -1294,7 +1303,7 @@
       <c r="B41">
         <v>4</v>
       </c>
-      <c r="C41" t="str">
+      <c r="C41" s="8" t="str">
         <f t="shared" si="0"/>
         <v>A4</v>
       </c>
@@ -1310,7 +1319,7 @@
       <c r="B42">
         <v>4</v>
       </c>
-      <c r="C42" t="str">
+      <c r="C42" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Ab4</v>
       </c>
@@ -1328,7 +1337,7 @@
       <c r="B43">
         <v>4</v>
       </c>
-      <c r="C43" t="str">
+      <c r="C43" s="8" t="str">
         <f t="shared" si="0"/>
         <v>G4</v>
       </c>
@@ -1348,7 +1357,7 @@
       <c r="B44">
         <v>4</v>
       </c>
-      <c r="C44" t="str">
+      <c r="C44" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Gb4</v>
       </c>
@@ -1368,7 +1377,7 @@
       <c r="B45">
         <v>4</v>
       </c>
-      <c r="C45" t="str">
+      <c r="C45" s="8" t="str">
         <f t="shared" si="0"/>
         <v>F4</v>
       </c>
@@ -1388,7 +1397,7 @@
       <c r="B46">
         <v>4</v>
       </c>
-      <c r="C46" t="str">
+      <c r="C46" s="8" t="str">
         <f t="shared" si="0"/>
         <v>E4</v>
       </c>
@@ -1407,7 +1416,7 @@
       <c r="B47">
         <v>4</v>
       </c>
-      <c r="C47" t="str">
+      <c r="C47" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Eb4</v>
       </c>
@@ -1427,7 +1436,7 @@
       <c r="B48">
         <v>4</v>
       </c>
-      <c r="C48" t="str">
+      <c r="C48" s="8" t="str">
         <f t="shared" si="0"/>
         <v>D4</v>
       </c>
@@ -1450,7 +1459,7 @@
       <c r="B49">
         <v>4</v>
       </c>
-      <c r="C49" t="str">
+      <c r="C49" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Db4</v>
       </c>
@@ -1469,7 +1478,7 @@
       <c r="B50">
         <v>3</v>
       </c>
-      <c r="C50" t="str">
+      <c r="C50" s="8" t="str">
         <f t="shared" si="0"/>
         <v>C3</v>
       </c>
@@ -1485,7 +1494,7 @@
       <c r="B51">
         <v>3</v>
       </c>
-      <c r="C51" t="str">
+      <c r="C51" s="8" t="str">
         <f t="shared" si="0"/>
         <v>B3</v>
       </c>
@@ -1502,7 +1511,7 @@
       <c r="B52">
         <v>3</v>
       </c>
-      <c r="C52" t="str">
+      <c r="C52" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Bb3</v>
       </c>
@@ -1519,7 +1528,7 @@
       <c r="B53">
         <v>3</v>
       </c>
-      <c r="C53" t="str">
+      <c r="C53" s="8" t="str">
         <f t="shared" si="0"/>
         <v>A3</v>
       </c>
@@ -1535,7 +1544,7 @@
       <c r="B54">
         <v>3</v>
       </c>
-      <c r="C54" t="str">
+      <c r="C54" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Ab3</v>
       </c>
@@ -1551,7 +1560,7 @@
       <c r="B55">
         <v>3</v>
       </c>
-      <c r="C55" t="str">
+      <c r="C55" s="8" t="str">
         <f t="shared" si="0"/>
         <v>G3</v>
       </c>
@@ -1566,7 +1575,7 @@
       <c r="B56">
         <v>3</v>
       </c>
-      <c r="C56" t="str">
+      <c r="C56" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Gb3</v>
       </c>
@@ -1581,7 +1590,7 @@
       <c r="B57">
         <v>3</v>
       </c>
-      <c r="C57" t="str">
+      <c r="C57" s="8" t="str">
         <f t="shared" si="0"/>
         <v>F3</v>
       </c>
@@ -1595,7 +1604,7 @@
       <c r="B58">
         <v>3</v>
       </c>
-      <c r="C58" t="str">
+      <c r="C58" s="8" t="str">
         <f t="shared" si="0"/>
         <v>E3</v>
       </c>
@@ -1608,7 +1617,7 @@
       <c r="B59">
         <v>3</v>
       </c>
-      <c r="C59" t="str">
+      <c r="C59" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Eb3</v>
       </c>
@@ -1623,7 +1632,7 @@
       <c r="B60">
         <v>3</v>
       </c>
-      <c r="C60" t="str">
+      <c r="C60" s="8" t="str">
         <f t="shared" si="0"/>
         <v>D3</v>
       </c>
@@ -1638,7 +1647,7 @@
       <c r="B61">
         <v>3</v>
       </c>
-      <c r="C61" t="str">
+      <c r="C61" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Db3</v>
       </c>
@@ -1652,7 +1661,7 @@
       <c r="B62">
         <v>2</v>
       </c>
-      <c r="C62" t="str">
+      <c r="C62" s="8" t="str">
         <f t="shared" si="0"/>
         <v>C2</v>
       </c>
@@ -1664,7 +1673,7 @@
       <c r="B63">
         <v>2</v>
       </c>
-      <c r="C63" t="str">
+      <c r="C63" s="8" t="str">
         <f t="shared" si="0"/>
         <v>B2</v>
       </c>
@@ -1676,7 +1685,7 @@
       <c r="B64">
         <v>2</v>
       </c>
-      <c r="C64" t="str">
+      <c r="C64" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Bb2</v>
       </c>
@@ -1690,7 +1699,7 @@
       <c r="B65">
         <v>2</v>
       </c>
-      <c r="C65" t="str">
+      <c r="C65" s="8" t="str">
         <f t="shared" si="0"/>
         <v>A2</v>
       </c>
@@ -1704,7 +1713,7 @@
       <c r="B66">
         <v>2</v>
       </c>
-      <c r="C66" t="str">
+      <c r="C66" s="8" t="str">
         <f t="shared" si="0"/>
         <v>Ab2</v>
       </c>
@@ -1720,7 +1729,7 @@
       <c r="B67">
         <v>2</v>
       </c>
-      <c r="C67" t="str">
+      <c r="C67" s="8" t="str">
         <f t="shared" ref="C67:C89" si="1">CONCATENATE(A67,B67)</f>
         <v>G2</v>
       </c>
@@ -1732,7 +1741,7 @@
       <c r="B68">
         <v>2</v>
       </c>
-      <c r="C68" t="str">
+      <c r="C68" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Gb2</v>
       </c>
@@ -1744,7 +1753,7 @@
       <c r="B69">
         <v>2</v>
       </c>
-      <c r="C69" t="str">
+      <c r="C69" s="8" t="str">
         <f t="shared" si="1"/>
         <v>F2</v>
       </c>
@@ -1756,7 +1765,7 @@
       <c r="B70">
         <v>2</v>
       </c>
-      <c r="C70" t="str">
+      <c r="C70" s="8" t="str">
         <f t="shared" si="1"/>
         <v>E2</v>
       </c>
@@ -1768,7 +1777,7 @@
       <c r="B71">
         <v>2</v>
       </c>
-      <c r="C71" t="str">
+      <c r="C71" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Eb2</v>
       </c>
@@ -1782,7 +1791,7 @@
       <c r="B72">
         <v>2</v>
       </c>
-      <c r="C72" t="str">
+      <c r="C72" s="8" t="str">
         <f t="shared" si="1"/>
         <v>D2</v>
       </c>
@@ -1796,7 +1805,7 @@
       <c r="B73">
         <v>2</v>
       </c>
-      <c r="C73" t="str">
+      <c r="C73" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Db2</v>
       </c>
@@ -1810,7 +1819,7 @@
       <c r="B74">
         <v>1</v>
       </c>
-      <c r="C74" t="str">
+      <c r="C74" s="8" t="str">
         <f t="shared" si="1"/>
         <v>C1</v>
       </c>
@@ -1822,7 +1831,7 @@
       <c r="B75">
         <v>1</v>
       </c>
-      <c r="C75" t="str">
+      <c r="C75" s="8" t="str">
         <f t="shared" si="1"/>
         <v>B1</v>
       </c>
@@ -1834,7 +1843,7 @@
       <c r="B76">
         <v>1</v>
       </c>
-      <c r="C76" t="str">
+      <c r="C76" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Bb1</v>
       </c>
@@ -1851,7 +1860,7 @@
       <c r="B77">
         <v>1</v>
       </c>
-      <c r="C77" t="str">
+      <c r="C77" s="8" t="str">
         <f t="shared" si="1"/>
         <v>A1</v>
       </c>
@@ -1865,7 +1874,7 @@
       <c r="B78">
         <v>1</v>
       </c>
-      <c r="C78" t="str">
+      <c r="C78" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Ab1</v>
       </c>
@@ -1879,7 +1888,7 @@
       <c r="B79">
         <v>1</v>
       </c>
-      <c r="C79" t="str">
+      <c r="C79" s="8" t="str">
         <f t="shared" si="1"/>
         <v>G1</v>
       </c>
@@ -1891,7 +1900,7 @@
       <c r="B80">
         <v>1</v>
       </c>
-      <c r="C80" t="str">
+      <c r="C80" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Gb1</v>
       </c>
@@ -1903,7 +1912,7 @@
       <c r="B81">
         <v>1</v>
       </c>
-      <c r="C81" t="str">
+      <c r="C81" s="8" t="str">
         <f t="shared" si="1"/>
         <v>F1</v>
       </c>
@@ -1915,7 +1924,7 @@
       <c r="B82">
         <v>1</v>
       </c>
-      <c r="C82" t="str">
+      <c r="C82" s="8" t="str">
         <f t="shared" si="1"/>
         <v>E1</v>
       </c>
@@ -1927,7 +1936,7 @@
       <c r="B83">
         <v>1</v>
       </c>
-      <c r="C83" t="str">
+      <c r="C83" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Eb1</v>
       </c>
@@ -1939,7 +1948,7 @@
       <c r="B84">
         <v>1</v>
       </c>
-      <c r="C84" t="str">
+      <c r="C84" s="8" t="str">
         <f t="shared" si="1"/>
         <v>D1</v>
       </c>
@@ -1951,7 +1960,7 @@
       <c r="B85">
         <v>1</v>
       </c>
-      <c r="C85" t="str">
+      <c r="C85" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Db1</v>
       </c>
@@ -1963,7 +1972,7 @@
       <c r="B86">
         <v>0</v>
       </c>
-      <c r="C86" t="str">
+      <c r="C86" s="8" t="str">
         <f t="shared" si="1"/>
         <v>C0</v>
       </c>
@@ -1975,7 +1984,7 @@
       <c r="B87">
         <v>0</v>
       </c>
-      <c r="C87" t="str">
+      <c r="C87" s="8" t="str">
         <f t="shared" si="1"/>
         <v>B0</v>
       </c>
@@ -1987,7 +1996,7 @@
       <c r="B88">
         <v>0</v>
       </c>
-      <c r="C88" t="str">
+      <c r="C88" s="8" t="str">
         <f t="shared" si="1"/>
         <v>Bb0</v>
       </c>
@@ -1999,14 +2008,13 @@
       <c r="B89">
         <v>0</v>
       </c>
-      <c r="C89" t="str">
+      <c r="C89" s="8" t="str">
         <f t="shared" si="1"/>
         <v>A0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="3" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
new figures for set klm
</commit_message>
<xml_diff>
--- a/figures/source/wald-register-space.xlsx
+++ b/figures/source/wald-register-space.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$C$1:$Q$78</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$C$1:$O$89</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -753,8 +753,8 @@
   </sheetPr>
   <dimension ref="A1:V94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="O1" sqref="D1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -762,14 +762,7 @@
     <col min="1" max="1" width="3.5" customWidth="1"/>
     <col min="2" max="2" width="2" customWidth="1"/>
     <col min="3" max="3" width="4.5" style="8" customWidth="1"/>
-    <col min="4" max="4" width="16.875" customWidth="1"/>
-    <col min="5" max="5" width="19.125" customWidth="1"/>
-    <col min="6" max="6" width="21.375" customWidth="1"/>
-    <col min="7" max="7" width="12.375" customWidth="1"/>
-    <col min="8" max="8" width="15.125" customWidth="1"/>
-    <col min="9" max="9" width="16.625" customWidth="1"/>
-    <col min="10" max="10" width="20.125" customWidth="1"/>
-    <col min="15" max="15" width="8.375" customWidth="1"/>
+    <col min="4" max="15" width="27.875" customWidth="1"/>
     <col min="16" max="16" width="37.875" customWidth="1"/>
     <col min="17" max="17" width="39.375" customWidth="1"/>
   </cols>
@@ -2112,7 +2105,7 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="3" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="3" scale="41" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>